<commit_message>
update get all new scema
modified scema get all
add api
</commit_message>
<xml_diff>
--- a/Dokumen/Progress.xlsx
+++ b/Dokumen/Progress.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="445" uniqueCount="184">
   <si>
     <t>Nama Table</t>
   </si>
@@ -471,10 +471,140 @@
     <t>Ok</t>
   </si>
   <si>
-    <t>Example</t>
-  </si>
-  <si>
     <t>andre</t>
+  </si>
+  <si>
+    <t>T_PurchaseReturn</t>
+  </si>
+  <si>
+    <t>T_PurchaseReturnDetail</t>
+  </si>
+  <si>
+    <t>T_SalesReturn</t>
+  </si>
+  <si>
+    <t>T_SalesReturnDetail</t>
+  </si>
+  <si>
+    <t>T_ReturnList</t>
+  </si>
+  <si>
+    <t>T_ReturnListDetail</t>
+  </si>
+  <si>
+    <t>T_waste</t>
+  </si>
+  <si>
+    <t>T_wasteDetail</t>
+  </si>
+  <si>
+    <t>pT_PurchaseReturn_View</t>
+  </si>
+  <si>
+    <t>pT_PurchaseReturn_Del</t>
+  </si>
+  <si>
+    <t>pT_PurchaseReturn_Bulk</t>
+  </si>
+  <si>
+    <t>pT_PurchaseReturnDetail_View</t>
+  </si>
+  <si>
+    <t>pT_SalesReturn_View</t>
+  </si>
+  <si>
+    <t>pT_SalesReturn_Bulk</t>
+  </si>
+  <si>
+    <t>pT_SalesReturnDetail_View</t>
+  </si>
+  <si>
+    <t>pT_ReturnList_View</t>
+  </si>
+  <si>
+    <t>pT_ReturnList_Del</t>
+  </si>
+  <si>
+    <t>pT_ReturnList_Bulk</t>
+  </si>
+  <si>
+    <t>pT_ReturnListDetail_View</t>
+  </si>
+  <si>
+    <t>pT_Waste_View</t>
+  </si>
+  <si>
+    <t>pT_Waste_Del</t>
+  </si>
+  <si>
+    <t>pT_Waste_Bulk</t>
+  </si>
+  <si>
+    <t>pT_WasteDetail_View</t>
+  </si>
+  <si>
+    <t>T_PurchaseReturn
+T_PurchaseReturnDetail</t>
+  </si>
+  <si>
+    <t>pT_SalesReturn_Del</t>
+  </si>
+  <si>
+    <t>T_SalesReturn
+T_SalesReturnDetail</t>
+  </si>
+  <si>
+    <t>T_ReturnList
+T_ReturnListDetail</t>
+  </si>
+  <si>
+    <t>T_WasteDetail</t>
+  </si>
+  <si>
+    <t>T_Waste
+T_WasteDetail</t>
+  </si>
+  <si>
+    <t>ok</t>
+  </si>
+  <si>
+    <t>pT_SODetail_Del</t>
+  </si>
+  <si>
+    <t>pT_GRDetail_Del</t>
+  </si>
+  <si>
+    <t>pT_DODetail_Del</t>
+  </si>
+  <si>
+    <t>pT_TransferDetail_Del</t>
+  </si>
+  <si>
+    <t>pM_Salesman_Del</t>
+  </si>
+  <si>
+    <t>pM_Supplier_Del</t>
+  </si>
+  <si>
+    <t>pT_PODetail_Del</t>
+  </si>
+  <si>
+    <t>pT_PermintaanBarangDetail_Del</t>
+  </si>
+  <si>
+    <t>pT_PengambilanBarangDetail_Del</t>
+  </si>
+  <si>
+    <t>pT_PurchaseReturnDetail_Del</t>
+  </si>
+  <si>
+    <t>pT_SalesReturnDetail_Del</t>
+  </si>
+  <si>
+    <t>pT_ReturnListDetail_Del</t>
+  </si>
+  <si>
+    <t>pT_WasteDetail_Del</t>
   </si>
 </sst>
 </file>
@@ -500,15 +630,21 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFD9D9D9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="5">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -576,11 +712,108 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -593,7 +826,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1"/>
@@ -601,12 +833,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -626,8 +852,71 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -950,13 +1239,13 @@
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="12">
+      <c r="A2" s="25">
         <v>1</v>
       </c>
-      <c r="B2" s="13" t="s">
+      <c r="B2" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="13" t="s">
+      <c r="C2" s="26" t="s">
         <v>17</v>
       </c>
       <c r="D2" t="s">
@@ -970,9 +1259,9 @@
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="12"/>
-      <c r="B3" s="13"/>
-      <c r="C3" s="13"/>
+      <c r="A3" s="25"/>
+      <c r="B3" s="26"/>
+      <c r="C3" s="26"/>
       <c r="D3" t="s">
         <v>13</v>
       </c>
@@ -984,9 +1273,9 @@
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="12"/>
-      <c r="B4" s="13"/>
-      <c r="C4" s="13"/>
+      <c r="A4" s="25"/>
+      <c r="B4" s="26"/>
+      <c r="C4" s="26"/>
       <c r="D4" t="s">
         <v>15</v>
       </c>
@@ -998,9 +1287,9 @@
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="12"/>
-      <c r="B5" s="13"/>
-      <c r="C5" s="13"/>
+      <c r="A5" s="25"/>
+      <c r="B5" s="26"/>
+      <c r="C5" s="26"/>
       <c r="D5" t="s">
         <v>11</v>
       </c>
@@ -1012,9 +1301,9 @@
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="12"/>
-      <c r="B6" s="13"/>
-      <c r="C6" s="13"/>
+      <c r="A6" s="25"/>
+      <c r="B6" s="26"/>
+      <c r="C6" s="26"/>
       <c r="D6" t="s">
         <v>12</v>
       </c>
@@ -1026,9 +1315,9 @@
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="12"/>
-      <c r="B7" s="13"/>
-      <c r="C7" s="13"/>
+      <c r="A7" s="25"/>
+      <c r="B7" s="26"/>
+      <c r="C7" s="26"/>
       <c r="D7" t="s">
         <v>14</v>
       </c>
@@ -1040,13 +1329,13 @@
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="12">
+      <c r="A8" s="25">
         <v>2</v>
       </c>
-      <c r="B8" s="13" t="s">
+      <c r="B8" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="13" t="s">
+      <c r="C8" s="26" t="s">
         <v>18</v>
       </c>
       <c r="D8" t="s">
@@ -1060,9 +1349,9 @@
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="12"/>
-      <c r="B9" s="13"/>
-      <c r="C9" s="13"/>
+      <c r="A9" s="25"/>
+      <c r="B9" s="26"/>
+      <c r="C9" s="26"/>
       <c r="D9" t="s">
         <v>13</v>
       </c>
@@ -1074,9 +1363,9 @@
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="12"/>
-      <c r="B10" s="13"/>
-      <c r="C10" s="13"/>
+      <c r="A10" s="25"/>
+      <c r="B10" s="26"/>
+      <c r="C10" s="26"/>
       <c r="D10" t="s">
         <v>15</v>
       </c>
@@ -1088,9 +1377,9 @@
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="12"/>
-      <c r="B11" s="13"/>
-      <c r="C11" s="13"/>
+      <c r="A11" s="25"/>
+      <c r="B11" s="26"/>
+      <c r="C11" s="26"/>
       <c r="D11" t="s">
         <v>11</v>
       </c>
@@ -1102,9 +1391,9 @@
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="12"/>
-      <c r="B12" s="13"/>
-      <c r="C12" s="13"/>
+      <c r="A12" s="25"/>
+      <c r="B12" s="26"/>
+      <c r="C12" s="26"/>
       <c r="D12" t="s">
         <v>12</v>
       </c>
@@ -1116,9 +1405,9 @@
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="12"/>
-      <c r="B13" s="13"/>
-      <c r="C13" s="13"/>
+      <c r="A13" s="25"/>
+      <c r="B13" s="26"/>
+      <c r="C13" s="26"/>
       <c r="D13" t="s">
         <v>14</v>
       </c>
@@ -1130,13 +1419,13 @@
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="12">
+      <c r="A14" s="25">
         <v>3</v>
       </c>
-      <c r="B14" s="13" t="s">
+      <c r="B14" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="C14" s="13" t="s">
+      <c r="C14" s="26" t="s">
         <v>19</v>
       </c>
       <c r="D14" t="s">
@@ -1150,9 +1439,9 @@
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="12"/>
-      <c r="B15" s="13"/>
-      <c r="C15" s="13"/>
+      <c r="A15" s="25"/>
+      <c r="B15" s="26"/>
+      <c r="C15" s="26"/>
       <c r="D15" t="s">
         <v>13</v>
       </c>
@@ -1164,9 +1453,9 @@
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="12"/>
-      <c r="B16" s="13"/>
-      <c r="C16" s="13"/>
+      <c r="A16" s="25"/>
+      <c r="B16" s="26"/>
+      <c r="C16" s="26"/>
       <c r="D16" t="s">
         <v>15</v>
       </c>
@@ -1178,9 +1467,9 @@
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="12"/>
-      <c r="B17" s="13"/>
-      <c r="C17" s="13"/>
+      <c r="A17" s="25"/>
+      <c r="B17" s="26"/>
+      <c r="C17" s="26"/>
       <c r="D17" t="s">
         <v>11</v>
       </c>
@@ -1192,9 +1481,9 @@
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="12"/>
-      <c r="B18" s="13"/>
-      <c r="C18" s="13"/>
+      <c r="A18" s="25"/>
+      <c r="B18" s="26"/>
+      <c r="C18" s="26"/>
       <c r="D18" t="s">
         <v>12</v>
       </c>
@@ -1206,9 +1495,9 @@
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="12"/>
-      <c r="B19" s="13"/>
-      <c r="C19" s="13"/>
+      <c r="A19" s="25"/>
+      <c r="B19" s="26"/>
+      <c r="C19" s="26"/>
       <c r="D19" t="s">
         <v>14</v>
       </c>
@@ -1220,13 +1509,13 @@
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="12">
+      <c r="A20" s="25">
         <v>4</v>
       </c>
-      <c r="B20" s="13" t="s">
+      <c r="B20" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="C20" s="13"/>
+      <c r="C20" s="26"/>
       <c r="D20" t="s">
         <v>10</v>
       </c>
@@ -1235,9 +1524,9 @@
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="12"/>
-      <c r="B21" s="13"/>
-      <c r="C21" s="13"/>
+      <c r="A21" s="25"/>
+      <c r="B21" s="26"/>
+      <c r="C21" s="26"/>
       <c r="D21" t="s">
         <v>13</v>
       </c>
@@ -1246,9 +1535,9 @@
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="12"/>
-      <c r="B22" s="13"/>
-      <c r="C22" s="13"/>
+      <c r="A22" s="25"/>
+      <c r="B22" s="26"/>
+      <c r="C22" s="26"/>
       <c r="D22" t="s">
         <v>15</v>
       </c>
@@ -1257,9 +1546,9 @@
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="12"/>
-      <c r="B23" s="13"/>
-      <c r="C23" s="13"/>
+      <c r="A23" s="25"/>
+      <c r="B23" s="26"/>
+      <c r="C23" s="26"/>
       <c r="D23" t="s">
         <v>11</v>
       </c>
@@ -1268,9 +1557,9 @@
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="12"/>
-      <c r="B24" s="13"/>
-      <c r="C24" s="13"/>
+      <c r="A24" s="25"/>
+      <c r="B24" s="26"/>
+      <c r="C24" s="26"/>
       <c r="D24" t="s">
         <v>12</v>
       </c>
@@ -1279,9 +1568,9 @@
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="12"/>
-      <c r="B25" s="13"/>
-      <c r="C25" s="13"/>
+      <c r="A25" s="25"/>
+      <c r="B25" s="26"/>
+      <c r="C25" s="26"/>
       <c r="D25" t="s">
         <v>14</v>
       </c>
@@ -1290,13 +1579,13 @@
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" s="12">
+      <c r="A26" s="25">
         <v>5</v>
       </c>
-      <c r="B26" s="13" t="s">
+      <c r="B26" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="C26" s="13"/>
+      <c r="C26" s="26"/>
       <c r="D26" t="s">
         <v>10</v>
       </c>
@@ -1305,9 +1594,9 @@
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" s="12"/>
-      <c r="B27" s="13"/>
-      <c r="C27" s="13"/>
+      <c r="A27" s="25"/>
+      <c r="B27" s="26"/>
+      <c r="C27" s="26"/>
       <c r="D27" t="s">
         <v>13</v>
       </c>
@@ -1316,9 +1605,9 @@
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" s="12"/>
-      <c r="B28" s="13"/>
-      <c r="C28" s="13"/>
+      <c r="A28" s="25"/>
+      <c r="B28" s="26"/>
+      <c r="C28" s="26"/>
       <c r="D28" t="s">
         <v>15</v>
       </c>
@@ -1327,9 +1616,9 @@
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" s="12"/>
-      <c r="B29" s="13"/>
-      <c r="C29" s="13"/>
+      <c r="A29" s="25"/>
+      <c r="B29" s="26"/>
+      <c r="C29" s="26"/>
       <c r="D29" t="s">
         <v>11</v>
       </c>
@@ -1338,9 +1627,9 @@
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30" s="12"/>
-      <c r="B30" s="13"/>
-      <c r="C30" s="13"/>
+      <c r="A30" s="25"/>
+      <c r="B30" s="26"/>
+      <c r="C30" s="26"/>
       <c r="D30" t="s">
         <v>12</v>
       </c>
@@ -1349,9 +1638,9 @@
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" s="12"/>
-      <c r="B31" s="13"/>
-      <c r="C31" s="13"/>
+      <c r="A31" s="25"/>
+      <c r="B31" s="26"/>
+      <c r="C31" s="26"/>
       <c r="D31" t="s">
         <v>14</v>
       </c>
@@ -1360,13 +1649,13 @@
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" s="12">
+      <c r="A32" s="25">
         <v>6</v>
       </c>
-      <c r="B32" s="13" t="s">
+      <c r="B32" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="C32" s="13"/>
+      <c r="C32" s="26"/>
       <c r="D32" t="s">
         <v>10</v>
       </c>
@@ -1375,9 +1664,9 @@
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33" s="12"/>
-      <c r="B33" s="13"/>
-      <c r="C33" s="13"/>
+      <c r="A33" s="25"/>
+      <c r="B33" s="26"/>
+      <c r="C33" s="26"/>
       <c r="D33" t="s">
         <v>13</v>
       </c>
@@ -1386,9 +1675,9 @@
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34" s="12"/>
-      <c r="B34" s="13"/>
-      <c r="C34" s="13"/>
+      <c r="A34" s="25"/>
+      <c r="B34" s="26"/>
+      <c r="C34" s="26"/>
       <c r="D34" t="s">
         <v>15</v>
       </c>
@@ -1397,9 +1686,9 @@
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A35" s="12"/>
-      <c r="B35" s="13"/>
-      <c r="C35" s="13"/>
+      <c r="A35" s="25"/>
+      <c r="B35" s="26"/>
+      <c r="C35" s="26"/>
       <c r="D35" t="s">
         <v>11</v>
       </c>
@@ -1408,9 +1697,9 @@
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A36" s="12"/>
-      <c r="B36" s="13"/>
-      <c r="C36" s="13"/>
+      <c r="A36" s="25"/>
+      <c r="B36" s="26"/>
+      <c r="C36" s="26"/>
       <c r="D36" t="s">
         <v>12</v>
       </c>
@@ -1419,9 +1708,9 @@
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A37" s="12"/>
-      <c r="B37" s="13"/>
-      <c r="C37" s="13"/>
+      <c r="A37" s="25"/>
+      <c r="B37" s="26"/>
+      <c r="C37" s="26"/>
       <c r="D37" t="s">
         <v>14</v>
       </c>
@@ -1431,24 +1720,24 @@
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="A26:A31"/>
+    <mergeCell ref="A32:A37"/>
+    <mergeCell ref="B26:B31"/>
+    <mergeCell ref="B32:B37"/>
+    <mergeCell ref="C32:C37"/>
+    <mergeCell ref="C26:C31"/>
+    <mergeCell ref="A14:A19"/>
+    <mergeCell ref="B14:B19"/>
+    <mergeCell ref="C14:C19"/>
+    <mergeCell ref="A20:A25"/>
+    <mergeCell ref="B20:B25"/>
+    <mergeCell ref="C20:C25"/>
     <mergeCell ref="A2:A7"/>
     <mergeCell ref="B2:B7"/>
     <mergeCell ref="C2:C7"/>
     <mergeCell ref="A8:A13"/>
     <mergeCell ref="B8:B13"/>
     <mergeCell ref="C8:C13"/>
-    <mergeCell ref="A14:A19"/>
-    <mergeCell ref="B14:B19"/>
-    <mergeCell ref="C14:C19"/>
-    <mergeCell ref="A20:A25"/>
-    <mergeCell ref="B20:B25"/>
-    <mergeCell ref="C20:C25"/>
-    <mergeCell ref="A26:A31"/>
-    <mergeCell ref="A32:A37"/>
-    <mergeCell ref="B26:B31"/>
-    <mergeCell ref="B32:B37"/>
-    <mergeCell ref="C32:C37"/>
-    <mergeCell ref="C26:C31"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="E2:E37">
@@ -1462,63 +1751,61 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F46"/>
+  <dimension ref="A1:F75"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="H41" sqref="H41"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A59" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A4" sqref="A4:A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.42578125" style="7" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.140625" style="7" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="33.28515625" style="7" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="32" style="7" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="9.140625" style="7"/>
+    <col min="1" max="1" width="26.42578125" style="6" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="33.28515625" style="6" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="32" style="6" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="7" t="s">
+    <row r="1" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="6" t="s">
         <v>112</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="E1" s="6" t="s">
         <v>138</v>
       </c>
-      <c r="F1" s="7" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" s="16" customFormat="1" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="15" t="s">
+    </row>
+    <row r="2" spans="1:5" s="13" customFormat="1" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="B2" s="15" t="s">
+      <c r="B2" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="C2" s="16" t="s">
+      <c r="C2" s="13" t="s">
         <v>69</v>
       </c>
-      <c r="D2" s="17" t="s">
+      <c r="D2" s="14" t="s">
         <v>113</v>
       </c>
-      <c r="E2" s="18" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" s="2" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="19" t="s">
+      <c r="E2" s="15" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" s="2" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="16" t="s">
         <v>44</v>
       </c>
-      <c r="B3" s="19" t="s">
+      <c r="B3" s="16" t="s">
         <v>48</v>
       </c>
       <c r="C3" s="2" t="s">
@@ -1527,15 +1814,15 @@
       <c r="D3" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="E3" s="20" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" s="2" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="19" t="s">
+      <c r="E3" s="17" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" s="2" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="30" t="s">
         <v>45</v>
       </c>
-      <c r="B4" s="19" t="s">
+      <c r="B4" s="16" t="s">
         <v>48</v>
       </c>
       <c r="C4" s="2" t="s">
@@ -1544,629 +1831,1184 @@
       <c r="D4" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="E4" s="20" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="8" t="s">
+      <c r="E4" s="17" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" s="18" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="32"/>
+      <c r="B5" s="16" t="s">
+        <v>49</v>
+      </c>
+      <c r="C5" s="18" t="s">
+        <v>176</v>
+      </c>
+      <c r="D5" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="E5" s="17" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="30" t="s">
         <v>46</v>
       </c>
-      <c r="B5" s="8" t="s">
+      <c r="B6" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="C5" s="7" t="s">
+      <c r="C6" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="D5" s="7" t="s">
+      <c r="D6" s="6" t="s">
         <v>114</v>
       </c>
-      <c r="E5" s="14" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="8" t="s">
+      <c r="E6" s="11" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="32"/>
+      <c r="B7" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>175</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="E7" s="11" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="37" t="s">
         <v>47</v>
       </c>
-      <c r="B6" s="8" t="s">
+      <c r="B8" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="C6" s="7" t="s">
+      <c r="C8" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="D6" s="11" t="s">
+      <c r="D8" s="10" t="s">
         <v>115</v>
       </c>
-      <c r="E6" s="14" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="8" t="s">
+      <c r="E8" s="11" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="38"/>
+      <c r="B9" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="C7" s="7" t="s">
+      <c r="C9" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="D7" s="7" t="s">
+      <c r="D9" s="6" t="s">
         <v>116</v>
       </c>
-      <c r="E7" s="14" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="8" t="s">
+      <c r="E9" s="11" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="39"/>
+      <c r="B10" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="C8" s="7" t="s">
+      <c r="C10" s="6" t="s">
         <v>75</v>
       </c>
-      <c r="D8" s="11" t="s">
+      <c r="D10" s="10" t="s">
         <v>117</v>
       </c>
-      <c r="E8" s="14" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="6" t="s">
+      <c r="E10" s="11" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="30" t="s">
         <v>51</v>
       </c>
-      <c r="B9" s="9" t="s">
+      <c r="B11" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="C9" s="7" t="s">
+      <c r="C11" s="6" t="s">
         <v>76</v>
       </c>
-      <c r="D9" s="7" t="s">
+      <c r="D11" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="E9" s="21" t="s">
+      <c r="E11" s="36" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="31"/>
+      <c r="B12" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="E12" s="36"/>
+    </row>
+    <row r="13" spans="1:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="31"/>
+      <c r="B13" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="D13" s="10" t="s">
+        <v>118</v>
+      </c>
+      <c r="E13" s="36"/>
+    </row>
+    <row r="14" spans="1:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="32"/>
+      <c r="B14" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="D14" s="10" t="s">
+        <v>119</v>
+      </c>
+      <c r="E14" s="36"/>
+    </row>
+    <row r="15" spans="1:5" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="30" t="s">
+        <v>53</v>
+      </c>
+      <c r="B15" s="23" t="s">
+        <v>48</v>
+      </c>
+      <c r="C15" s="18" t="s">
+        <v>80</v>
+      </c>
+      <c r="D15" s="10" t="s">
+        <v>120</v>
+      </c>
+      <c r="E15" s="36"/>
+    </row>
+    <row r="16" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="32"/>
+      <c r="B16" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>177</v>
+      </c>
+      <c r="D16" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="E16" s="22" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="30" t="s">
+        <v>54</v>
+      </c>
+      <c r="B17" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="D17" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="E17" s="11" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="31"/>
+      <c r="B18" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="C18" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="D18" s="10" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="31"/>
+      <c r="B19" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="C19" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="D19" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="E19" s="11" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="32"/>
+      <c r="B20" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="C20" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="D20" s="10" t="s">
+        <v>122</v>
+      </c>
+      <c r="E20" s="11" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="30" t="s">
+        <v>55</v>
+      </c>
+      <c r="B21" s="23" t="s">
+        <v>48</v>
+      </c>
+      <c r="C21" s="18" t="s">
+        <v>86</v>
+      </c>
+      <c r="D21" s="10" t="s">
+        <v>123</v>
+      </c>
+      <c r="E21" s="11" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="32"/>
+      <c r="B22" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="C22" s="6" t="s">
+        <v>171</v>
+      </c>
+      <c r="D22" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="E22" s="11" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="30" t="s">
+        <v>56</v>
+      </c>
+      <c r="B23" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="C23" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="D23" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="E23" s="11" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="31"/>
+      <c r="B24" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="C24" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="D24" s="10" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="31"/>
+      <c r="B25" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="C25" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="D25" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="E25" s="11" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="32"/>
+      <c r="B26" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="C26" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="D26" s="10" t="s">
+        <v>124</v>
+      </c>
+      <c r="E26" s="11" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="30" t="s">
+        <v>57</v>
+      </c>
+      <c r="B27" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="C27" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="D27" s="10" t="s">
+        <v>125</v>
+      </c>
+      <c r="E27" s="11" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="32"/>
+      <c r="B28" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="C28" s="6" t="s">
+        <v>172</v>
+      </c>
+      <c r="D28" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="E28" s="11" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="30" t="s">
+        <v>58</v>
+      </c>
+      <c r="B29" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="C29" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="D29" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="E29" s="11" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="31"/>
+      <c r="B30" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="C30" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="D30" s="10" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="31"/>
+      <c r="B31" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="C31" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="D31" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="E31" s="11" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="32"/>
+      <c r="B32" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="C32" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="D32" s="10" t="s">
+        <v>126</v>
+      </c>
+      <c r="E32" s="11" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="30" t="s">
+        <v>59</v>
+      </c>
+      <c r="B33" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="C33" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="D33" s="10" t="s">
+        <v>127</v>
+      </c>
+      <c r="E33" s="11" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="32"/>
+      <c r="B34" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="C34" s="6" t="s">
+        <v>173</v>
+      </c>
+      <c r="D34" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="E34" s="11" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="30" t="s">
+        <v>60</v>
+      </c>
+      <c r="B35" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="C35" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="D35" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="E35" s="11" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="31"/>
+      <c r="B36" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="C36" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="D36" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="E36" s="11" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="31"/>
+      <c r="B37" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="C37" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="D37" s="10" t="s">
+        <v>128</v>
+      </c>
+      <c r="E37" s="11" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="32"/>
+      <c r="B38" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="C38" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="D38" s="10" t="s">
+        <v>129</v>
+      </c>
+      <c r="E38" s="11" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="30" t="s">
+        <v>61</v>
+      </c>
+      <c r="B39" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="C39" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="D39" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="E39" s="11" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="32"/>
+      <c r="B40" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="C40" s="6" t="s">
+        <v>174</v>
+      </c>
+      <c r="D40" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="E40" s="11" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="30" t="s">
+        <v>62</v>
+      </c>
+      <c r="B41" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="C41" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="D41" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="E41" s="11" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="31"/>
+      <c r="B42" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="C42" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="D42" s="6" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="31"/>
+      <c r="B43" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="C43" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="D43" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="E43" s="11" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="32"/>
+      <c r="B44" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="C44" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="D44" s="10" t="s">
+        <v>130</v>
+      </c>
+      <c r="E44" s="11" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A45" s="30" t="s">
+        <v>63</v>
+      </c>
+      <c r="B45" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="C45" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="D45" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="E45" s="11" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="32"/>
+      <c r="B46" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="C46" s="6" t="s">
+        <v>178</v>
+      </c>
+      <c r="D46" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="E46" s="11" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="30" t="s">
+        <v>64</v>
+      </c>
+      <c r="B47" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="C47" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="D47" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="E47" s="11" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A48" s="31"/>
+      <c r="B48" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="C48" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="D48" s="6" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A49" s="31"/>
+      <c r="B49" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="C49" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="D49" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="E49" s="11" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A50" s="32"/>
+      <c r="B50" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="C50" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="D50" s="10" t="s">
+        <v>131</v>
+      </c>
+      <c r="E50" s="11" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A51" s="33" t="s">
+        <v>65</v>
+      </c>
+      <c r="B51" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="C51" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="D51" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="E51" s="11" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A52" s="34"/>
+      <c r="B52" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="C52" s="6" t="s">
+        <v>179</v>
+      </c>
+      <c r="D52" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="E52" s="11" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A53" s="26" t="s">
+        <v>132</v>
+      </c>
+      <c r="B53" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="C53" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="D53" s="6" t="s">
+        <v>132</v>
+      </c>
+      <c r="E53" s="11" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A54" s="26"/>
+      <c r="B54" s="6" t="s">
+        <v>134</v>
+      </c>
+      <c r="C54" s="6" t="s">
+        <v>136</v>
+      </c>
+      <c r="D54" s="6" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A55" s="35"/>
+      <c r="B55" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="C55" s="6" t="s">
+        <v>137</v>
+      </c>
+      <c r="D55" s="6" t="s">
+        <v>132</v>
+      </c>
+      <c r="E55" s="6" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A56" s="27" t="s">
         <v>141</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="8"/>
-      <c r="B10" s="10" t="s">
-        <v>52</v>
-      </c>
-      <c r="C10" s="7" t="s">
-        <v>77</v>
-      </c>
-      <c r="D10" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="E10" s="21"/>
-    </row>
-    <row r="11" spans="1:6" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="8"/>
-      <c r="B11" s="10" t="s">
+      <c r="B56" s="19" t="s">
+        <v>48</v>
+      </c>
+      <c r="C56" s="6" t="s">
+        <v>149</v>
+      </c>
+      <c r="D56" s="6" t="s">
+        <v>141</v>
+      </c>
+      <c r="E56" s="6" t="s">
+        <v>139</v>
+      </c>
+      <c r="F56" s="11" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A57" s="28"/>
+      <c r="B57" s="21" t="s">
         <v>49</v>
       </c>
-      <c r="C11" s="7" t="s">
-        <v>78</v>
-      </c>
-      <c r="D11" s="11" t="s">
-        <v>118</v>
-      </c>
-      <c r="E11" s="21"/>
-    </row>
-    <row r="12" spans="1:6" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="8"/>
-      <c r="B12" s="10" t="s">
+      <c r="C57" s="6" t="s">
+        <v>150</v>
+      </c>
+      <c r="D57" s="10" t="s">
+        <v>164</v>
+      </c>
+      <c r="E57" s="6" t="s">
+        <v>139</v>
+      </c>
+      <c r="F57" s="6" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A58" s="29"/>
+      <c r="B58" s="21" t="s">
         <v>50</v>
       </c>
-      <c r="C12" s="7" t="s">
-        <v>79</v>
-      </c>
-      <c r="D12" s="11" t="s">
-        <v>119</v>
-      </c>
-      <c r="E12" s="21"/>
-    </row>
-    <row r="13" spans="1:6" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="B13" s="10" t="s">
+      <c r="C58" s="6" t="s">
+        <v>151</v>
+      </c>
+      <c r="D58" s="10" t="s">
+        <v>164</v>
+      </c>
+      <c r="E58" s="6" t="s">
+        <v>139</v>
+      </c>
+      <c r="F58" s="6" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A59" s="27" t="s">
+        <v>142</v>
+      </c>
+      <c r="B59" s="21" t="s">
         <v>48</v>
       </c>
-      <c r="C13" s="7" t="s">
-        <v>80</v>
-      </c>
-      <c r="D13" s="11" t="s">
-        <v>120</v>
-      </c>
-      <c r="E13" s="21"/>
-    </row>
-    <row r="14" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="8" t="s">
-        <v>54</v>
-      </c>
-      <c r="B14" s="10" t="s">
+      <c r="C59" s="6" t="s">
+        <v>152</v>
+      </c>
+      <c r="D59" s="6" t="s">
+        <v>142</v>
+      </c>
+      <c r="E59" s="6" t="s">
+        <v>139</v>
+      </c>
+      <c r="F59" s="11" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A60" s="29"/>
+      <c r="B60" s="21" t="s">
+        <v>49</v>
+      </c>
+      <c r="C60" s="6" t="s">
+        <v>180</v>
+      </c>
+      <c r="D60" s="6" t="s">
+        <v>142</v>
+      </c>
+      <c r="E60" s="6" t="s">
+        <v>139</v>
+      </c>
+      <c r="F60" s="11" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A61" s="27" t="s">
+        <v>143</v>
+      </c>
+      <c r="B61" s="21" t="s">
         <v>48</v>
       </c>
-      <c r="C14" s="7" t="s">
-        <v>81</v>
-      </c>
-      <c r="D14" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="E14" s="14" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="8"/>
-      <c r="B15" s="10" t="s">
-        <v>52</v>
-      </c>
-      <c r="C15" s="7" t="s">
-        <v>82</v>
-      </c>
-      <c r="D15" s="11" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="8"/>
-      <c r="B16" s="10" t="s">
+      <c r="C61" s="6" t="s">
+        <v>153</v>
+      </c>
+      <c r="D61" s="6" t="s">
+        <v>143</v>
+      </c>
+      <c r="E61" s="6" t="s">
+        <v>139</v>
+      </c>
+      <c r="F61" s="11" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A62" s="28"/>
+      <c r="B62" s="21" t="s">
         <v>49</v>
       </c>
-      <c r="C16" s="7" t="s">
-        <v>83</v>
-      </c>
-      <c r="D16" s="11" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="8"/>
-      <c r="B17" s="10" t="s">
-        <v>84</v>
-      </c>
-      <c r="C17" s="7" t="s">
-        <v>85</v>
-      </c>
-      <c r="D17" s="11" t="s">
-        <v>122</v>
-      </c>
-      <c r="E17" s="14" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="8" t="s">
-        <v>55</v>
-      </c>
-      <c r="B18" s="10" t="s">
+      <c r="C62" s="6" t="s">
+        <v>165</v>
+      </c>
+      <c r="D62" s="10" t="s">
+        <v>166</v>
+      </c>
+      <c r="E62" s="6" t="s">
+        <v>139</v>
+      </c>
+      <c r="F62" s="6" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A63" s="29"/>
+      <c r="B63" s="21" t="s">
+        <v>50</v>
+      </c>
+      <c r="C63" s="6" t="s">
+        <v>154</v>
+      </c>
+      <c r="D63" s="10" t="s">
+        <v>166</v>
+      </c>
+      <c r="E63" s="6" t="s">
+        <v>139</v>
+      </c>
+      <c r="F63" s="6" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A64" s="27" t="s">
+        <v>144</v>
+      </c>
+      <c r="B64" s="21" t="s">
         <v>48</v>
       </c>
-      <c r="C18" s="7" t="s">
-        <v>86</v>
-      </c>
-      <c r="D18" s="11" t="s">
-        <v>123</v>
-      </c>
-      <c r="E18" s="14" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="B19" s="10" t="s">
+      <c r="C64" s="6" t="s">
+        <v>155</v>
+      </c>
+      <c r="D64" s="6" t="s">
+        <v>144</v>
+      </c>
+      <c r="E64" s="6" t="s">
+        <v>139</v>
+      </c>
+      <c r="F64" s="11" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A65" s="29"/>
+      <c r="B65" s="21" t="s">
+        <v>49</v>
+      </c>
+      <c r="C65" s="6" t="s">
+        <v>181</v>
+      </c>
+      <c r="D65" s="6" t="s">
+        <v>144</v>
+      </c>
+      <c r="E65" s="6" t="s">
+        <v>139</v>
+      </c>
+      <c r="F65" s="11" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A66" s="27" t="s">
+        <v>145</v>
+      </c>
+      <c r="B66" s="21" t="s">
         <v>48</v>
       </c>
-      <c r="C19" s="7" t="s">
-        <v>87</v>
-      </c>
-      <c r="D19" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="E19" s="14" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="8"/>
-      <c r="B20" s="10" t="s">
-        <v>52</v>
-      </c>
-      <c r="C20" s="7" t="s">
-        <v>88</v>
-      </c>
-      <c r="D20" s="11" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="8"/>
-      <c r="B21" s="10" t="s">
+      <c r="C66" s="6" t="s">
+        <v>156</v>
+      </c>
+      <c r="D66" s="6" t="s">
+        <v>145</v>
+      </c>
+      <c r="E66" s="6" t="s">
+        <v>139</v>
+      </c>
+      <c r="F66" s="11" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A67" s="28"/>
+      <c r="B67" s="21" t="s">
         <v>49</v>
       </c>
-      <c r="C21" s="7" t="s">
-        <v>89</v>
-      </c>
-      <c r="D21" s="11" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="8"/>
-      <c r="B22" s="10" t="s">
+      <c r="C67" s="6" t="s">
+        <v>157</v>
+      </c>
+      <c r="D67" s="10" t="s">
+        <v>167</v>
+      </c>
+      <c r="E67" s="6" t="s">
+        <v>139</v>
+      </c>
+      <c r="F67" s="6" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A68" s="29"/>
+      <c r="B68" s="21" t="s">
         <v>50</v>
       </c>
-      <c r="C22" s="7" t="s">
-        <v>90</v>
-      </c>
-      <c r="D22" s="11" t="s">
-        <v>124</v>
-      </c>
-      <c r="E22" s="14" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="8" t="s">
-        <v>57</v>
-      </c>
-      <c r="B23" s="10" t="s">
+      <c r="C68" s="6" t="s">
+        <v>158</v>
+      </c>
+      <c r="D68" s="10" t="s">
+        <v>167</v>
+      </c>
+      <c r="E68" s="6" t="s">
+        <v>139</v>
+      </c>
+      <c r="F68" s="6" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A69" s="20" t="s">
+        <v>146</v>
+      </c>
+      <c r="B69" s="21" t="s">
         <v>48</v>
       </c>
-      <c r="C23" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="D23" s="11" t="s">
-        <v>125</v>
-      </c>
-      <c r="E23" s="14" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="8" t="s">
-        <v>58</v>
-      </c>
-      <c r="B24" s="10" t="s">
+      <c r="C69" s="6" t="s">
+        <v>159</v>
+      </c>
+      <c r="D69" s="6" t="s">
+        <v>146</v>
+      </c>
+      <c r="E69" s="6" t="s">
+        <v>170</v>
+      </c>
+      <c r="F69" s="11" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A70" s="20"/>
+      <c r="B70" s="21" t="s">
+        <v>49</v>
+      </c>
+      <c r="C70" s="6" t="s">
+        <v>182</v>
+      </c>
+      <c r="D70" s="6" t="s">
+        <v>146</v>
+      </c>
+      <c r="E70" s="6" t="s">
+        <v>170</v>
+      </c>
+      <c r="F70" s="11" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A71" s="20" t="s">
+        <v>147</v>
+      </c>
+      <c r="B71" s="21" t="s">
         <v>48</v>
       </c>
-      <c r="C24" s="7" t="s">
-        <v>92</v>
-      </c>
-      <c r="D24" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="E24" s="14" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="8"/>
-      <c r="B25" s="10" t="s">
-        <v>52</v>
-      </c>
-      <c r="C25" s="7" t="s">
-        <v>93</v>
-      </c>
-      <c r="D25" s="11" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="8"/>
-      <c r="B26" s="10" t="s">
+      <c r="C71" s="6" t="s">
+        <v>160</v>
+      </c>
+      <c r="D71" s="10" t="s">
+        <v>169</v>
+      </c>
+      <c r="E71" s="6" t="s">
+        <v>139</v>
+      </c>
+      <c r="F71" s="6" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A72" s="20"/>
+      <c r="B72" s="21" t="s">
         <v>49</v>
       </c>
-      <c r="C26" s="7" t="s">
-        <v>94</v>
-      </c>
-      <c r="D26" s="11" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="8"/>
-      <c r="B27" s="10" t="s">
+      <c r="C72" s="6" t="s">
+        <v>161</v>
+      </c>
+      <c r="D72" s="10" t="s">
+        <v>169</v>
+      </c>
+      <c r="E72" s="6" t="s">
+        <v>139</v>
+      </c>
+      <c r="F72" s="6" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A73" s="20"/>
+      <c r="B73" s="21" t="s">
         <v>50</v>
       </c>
-      <c r="C27" s="7" t="s">
-        <v>95</v>
-      </c>
-      <c r="D27" s="11" t="s">
-        <v>126</v>
-      </c>
-      <c r="E27" s="14" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="8" t="s">
-        <v>59</v>
-      </c>
-      <c r="B28" s="10" t="s">
+      <c r="C73" s="6" t="s">
+        <v>162</v>
+      </c>
+      <c r="D73" s="10" t="s">
+        <v>169</v>
+      </c>
+      <c r="E73" s="6" t="s">
+        <v>139</v>
+      </c>
+      <c r="F73" s="6" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A74" s="20" t="s">
+        <v>148</v>
+      </c>
+      <c r="B74" s="21" t="s">
         <v>48</v>
       </c>
-      <c r="C28" s="7" t="s">
-        <v>96</v>
-      </c>
-      <c r="D28" s="11" t="s">
-        <v>127</v>
-      </c>
-      <c r="E28" s="14" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="8" t="s">
-        <v>60</v>
-      </c>
-      <c r="B29" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="C29" s="7" t="s">
-        <v>97</v>
-      </c>
-      <c r="D29" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="E29" s="14" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="8"/>
-      <c r="B30" s="10" t="s">
-        <v>52</v>
-      </c>
-      <c r="C30" s="7" t="s">
-        <v>98</v>
-      </c>
-      <c r="D30" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="E30" s="14" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="8"/>
-      <c r="B31" s="10" t="s">
+      <c r="C74" s="6" t="s">
+        <v>163</v>
+      </c>
+      <c r="D74" s="6" t="s">
+        <v>168</v>
+      </c>
+      <c r="E74" s="6" t="s">
+        <v>139</v>
+      </c>
+      <c r="F74" s="11" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B75" s="24" t="s">
         <v>49</v>
       </c>
-      <c r="C31" s="7" t="s">
-        <v>99</v>
-      </c>
-      <c r="D31" s="11" t="s">
-        <v>128</v>
-      </c>
-      <c r="E31" s="14" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="8"/>
-      <c r="B32" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="C32" s="7" t="s">
-        <v>100</v>
-      </c>
-      <c r="D32" s="11" t="s">
-        <v>129</v>
-      </c>
-      <c r="E32" s="14" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="8" t="s">
-        <v>61</v>
-      </c>
-      <c r="B33" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="C33" s="7" t="s">
-        <v>101</v>
-      </c>
-      <c r="D33" s="7" t="s">
-        <v>61</v>
-      </c>
-      <c r="E33" s="14" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="8" t="s">
-        <v>62</v>
-      </c>
-      <c r="B34" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="C34" s="7" t="s">
-        <v>102</v>
-      </c>
-      <c r="D34" s="7" t="s">
-        <v>62</v>
-      </c>
-      <c r="E34" s="14" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="8"/>
-      <c r="B35" s="10" t="s">
-        <v>52</v>
-      </c>
-      <c r="C35" s="7" t="s">
-        <v>103</v>
-      </c>
-      <c r="D35" s="7" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="8"/>
-      <c r="B36" s="10" t="s">
-        <v>49</v>
-      </c>
-      <c r="C36" s="7" t="s">
-        <v>104</v>
-      </c>
-      <c r="D36" s="7" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="8"/>
-      <c r="B37" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="C37" s="7" t="s">
-        <v>105</v>
-      </c>
-      <c r="D37" s="11" t="s">
-        <v>130</v>
-      </c>
-      <c r="E37" s="14" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="B38" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="C38" s="7" t="s">
-        <v>106</v>
-      </c>
-      <c r="D38" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="E38" s="14" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="8" t="s">
-        <v>64</v>
-      </c>
-      <c r="B39" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="C39" s="7" t="s">
-        <v>107</v>
-      </c>
-      <c r="D39" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="E39" s="14" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="8"/>
-      <c r="B40" s="10" t="s">
-        <v>52</v>
-      </c>
-      <c r="C40" s="7" t="s">
-        <v>108</v>
-      </c>
-      <c r="D40" s="7" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="8"/>
-      <c r="B41" s="10" t="s">
-        <v>49</v>
-      </c>
-      <c r="C41" s="7" t="s">
-        <v>109</v>
-      </c>
-      <c r="D41" s="7" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="8"/>
-      <c r="B42" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="C42" s="7" t="s">
-        <v>110</v>
-      </c>
-      <c r="D42" s="11" t="s">
-        <v>131</v>
-      </c>
-      <c r="E42" s="14" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="8" t="s">
-        <v>65</v>
-      </c>
-      <c r="B43" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="C43" s="7" t="s">
-        <v>111</v>
-      </c>
-      <c r="D43" s="7" t="s">
-        <v>65</v>
-      </c>
-      <c r="E43" s="14" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="7" t="s">
-        <v>132</v>
-      </c>
-      <c r="B44" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="C44" s="7" t="s">
-        <v>133</v>
-      </c>
-      <c r="D44" s="7" t="s">
-        <v>132</v>
-      </c>
-      <c r="E44" s="14" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B45" s="7" t="s">
-        <v>134</v>
-      </c>
-      <c r="C45" s="7" t="s">
-        <v>136</v>
-      </c>
-      <c r="D45" s="7" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B46" s="7" t="s">
-        <v>135</v>
-      </c>
-      <c r="C46" s="7" t="s">
-        <v>137</v>
-      </c>
-      <c r="D46" s="7" t="s">
-        <v>121</v>
+      <c r="C75" s="6" t="s">
+        <v>183</v>
+      </c>
+      <c r="D75" s="6" t="s">
+        <v>168</v>
+      </c>
+      <c r="E75" s="11" t="s">
+        <v>139</v>
+      </c>
+      <c r="F75" s="11" t="s">
+        <v>139</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="E9:E13"/>
+  <mergeCells count="24">
+    <mergeCell ref="E11:E15"/>
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="A8:A10"/>
+    <mergeCell ref="A11:A14"/>
+    <mergeCell ref="A15:A16"/>
+    <mergeCell ref="A17:A20"/>
+    <mergeCell ref="A21:A22"/>
+    <mergeCell ref="A23:A26"/>
+    <mergeCell ref="A27:A28"/>
+    <mergeCell ref="A29:A32"/>
+    <mergeCell ref="A33:A34"/>
+    <mergeCell ref="A35:A38"/>
+    <mergeCell ref="A39:A40"/>
+    <mergeCell ref="A41:A44"/>
+    <mergeCell ref="A45:A46"/>
+    <mergeCell ref="A61:A63"/>
+    <mergeCell ref="A64:A65"/>
+    <mergeCell ref="A66:A68"/>
+    <mergeCell ref="A47:A50"/>
+    <mergeCell ref="A51:A52"/>
+    <mergeCell ref="A53:A55"/>
+    <mergeCell ref="A56:A58"/>
+    <mergeCell ref="A59:A60"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>